<commit_message>
correção no trecho de comparação de meses
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\Projetos\estatisticas_iten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17D411A-65B1-4BAF-A782-210CE68228AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E99846B-D0A4-4F58-A738-9FC4B172D5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -159,10 +159,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,6 +233,7 @@
           <cell r="N41" t="str">
             <v>REP</v>
           </cell>
+          <cell r="O41"/>
           <cell r="P41">
             <v>8</v>
           </cell>
@@ -255,11 +252,18 @@
           <cell r="U41">
             <v>26</v>
           </cell>
+          <cell r="V41"/>
+          <cell r="W41"/>
+          <cell r="X41"/>
+          <cell r="Y41"/>
+          <cell r="Z41"/>
+          <cell r="AA41"/>
         </row>
         <row r="42">
           <cell r="N42" t="str">
             <v>Técnico</v>
           </cell>
+          <cell r="O42"/>
           <cell r="P42">
             <v>33</v>
           </cell>
@@ -278,6 +282,12 @@
           <cell r="U42">
             <v>60</v>
           </cell>
+          <cell r="V42"/>
+          <cell r="W42"/>
+          <cell r="X42"/>
+          <cell r="Y42"/>
+          <cell r="Z42"/>
+          <cell r="AA42"/>
         </row>
       </sheetData>
       <sheetData sheetId="3">
@@ -299,93 +309,117 @@
           <cell r="F8" t="str">
             <v>REP</v>
           </cell>
-          <cell r="G8">
+          <cell r="G8"/>
+          <cell r="H8">
             <v>5</v>
           </cell>
-          <cell r="H8">
+          <cell r="I8">
             <v>10</v>
           </cell>
-          <cell r="I8">
+          <cell r="J8">
             <v>2</v>
           </cell>
-          <cell r="J8">
+          <cell r="K8">
             <v>6</v>
           </cell>
-          <cell r="K8">
+          <cell r="L8">
             <v>11</v>
           </cell>
-          <cell r="L8">
+          <cell r="M8">
             <v>9</v>
           </cell>
+          <cell r="N8"/>
+          <cell r="O8"/>
+          <cell r="P8"/>
+          <cell r="Q8"/>
+          <cell r="R8"/>
         </row>
         <row r="9">
           <cell r="F9" t="str">
             <v>Técnico</v>
           </cell>
-          <cell r="G9">
+          <cell r="G9"/>
+          <cell r="H9">
             <v>10</v>
           </cell>
-          <cell r="H9">
+          <cell r="I9">
             <v>7</v>
           </cell>
-          <cell r="I9">
+          <cell r="J9">
             <v>16</v>
           </cell>
-          <cell r="J9">
+          <cell r="K9">
             <v>4</v>
           </cell>
-          <cell r="K9">
+          <cell r="L9">
             <v>12</v>
           </cell>
-          <cell r="L9">
+          <cell r="M9">
             <v>14</v>
           </cell>
+          <cell r="N9"/>
+          <cell r="O9"/>
+          <cell r="P9"/>
+          <cell r="Q9"/>
+          <cell r="R9"/>
         </row>
         <row r="10">
           <cell r="F10" t="str">
             <v>Comercial</v>
           </cell>
-          <cell r="G10">
+          <cell r="G10"/>
+          <cell r="H10">
             <v>22</v>
           </cell>
-          <cell r="H10">
+          <cell r="I10">
             <v>6</v>
           </cell>
-          <cell r="I10">
+          <cell r="J10">
             <v>2</v>
           </cell>
-          <cell r="J10">
+          <cell r="K10">
             <v>3</v>
           </cell>
-          <cell r="K10">
+          <cell r="L10">
             <v>2</v>
           </cell>
-          <cell r="L10">
+          <cell r="M10">
             <v>7</v>
           </cell>
+          <cell r="N10"/>
+          <cell r="O10"/>
+          <cell r="P10"/>
+          <cell r="Q10"/>
+          <cell r="R10"/>
         </row>
         <row r="11">
           <cell r="F11" t="str">
             <v>Cliente</v>
           </cell>
-          <cell r="G11">
+          <cell r="G11"/>
+          <cell r="H11">
             <v>14</v>
           </cell>
-          <cell r="H11">
+          <cell r="I11">
             <v>10</v>
           </cell>
-          <cell r="I11">
+          <cell r="J11">
             <v>13</v>
           </cell>
-          <cell r="J11">
+          <cell r="K11">
             <v>8</v>
           </cell>
-          <cell r="K11">
+          <cell r="L11">
             <v>9</v>
           </cell>
-          <cell r="L11">
+          <cell r="M11">
             <v>15</v>
           </cell>
+          <cell r="N11"/>
+          <cell r="O11"/>
+          <cell r="P11"/>
+          <cell r="Q11"/>
+          <cell r="R11"/>
         </row>
       </sheetData>
       <sheetData sheetId="4">
@@ -421,78 +455,97 @@
           <cell r="G8" t="str">
             <v>Bruna</v>
           </cell>
-          <cell r="H8">
+          <cell r="H8"/>
+          <cell r="I8">
             <v>5</v>
           </cell>
-          <cell r="I8">
+          <cell r="J8">
             <v>13</v>
           </cell>
-          <cell r="J8">
+          <cell r="K8">
             <v>19</v>
           </cell>
-          <cell r="K8">
+          <cell r="L8">
             <v>13</v>
           </cell>
-          <cell r="L8">
+          <cell r="M8">
             <v>136</v>
           </cell>
-          <cell r="M8">
+          <cell r="N8">
             <v>100</v>
           </cell>
+          <cell r="O8"/>
+          <cell r="P8"/>
+          <cell r="Q8"/>
+          <cell r="R8"/>
+          <cell r="S8"/>
+          <cell r="T8"/>
         </row>
         <row r="9">
           <cell r="G9" t="str">
             <v>Elias</v>
           </cell>
-          <cell r="H9">
+          <cell r="H9"/>
+          <cell r="I9">
             <v>36</v>
           </cell>
-          <cell r="I9">
+          <cell r="J9">
             <v>37</v>
           </cell>
-          <cell r="J9">
+          <cell r="K9">
             <v>43</v>
           </cell>
-          <cell r="K9">
+          <cell r="L9">
             <v>50</v>
           </cell>
-          <cell r="L9">
+          <cell r="M9">
             <v>65</v>
           </cell>
-          <cell r="M9">
+          <cell r="N9">
             <v>59</v>
           </cell>
+          <cell r="O9"/>
+          <cell r="P9"/>
+          <cell r="Q9"/>
+          <cell r="R9"/>
+          <cell r="S9"/>
+          <cell r="T9"/>
         </row>
         <row r="10">
           <cell r="G10" t="str">
             <v>Marcel</v>
           </cell>
-          <cell r="H10">
+          <cell r="H10"/>
+          <cell r="I10">
             <v>11</v>
           </cell>
-          <cell r="I10">
+          <cell r="J10">
             <v>29</v>
           </cell>
-          <cell r="J10">
+          <cell r="K10">
             <v>46</v>
           </cell>
-          <cell r="K10">
+          <cell r="L10">
             <v>28</v>
           </cell>
-          <cell r="L10">
+          <cell r="M10">
             <v>127</v>
           </cell>
-          <cell r="M10">
+          <cell r="N10">
             <v>61</v>
           </cell>
+          <cell r="O10"/>
+          <cell r="P10"/>
+          <cell r="Q10"/>
+          <cell r="R10"/>
+          <cell r="S10"/>
+          <cell r="T10"/>
         </row>
         <row r="11">
           <cell r="G11" t="str">
             <v>Vitoria</v>
           </cell>
-          <cell r="H11">
-            <v>0</v>
-          </cell>
+          <cell r="H11"/>
           <cell r="I11">
             <v>0</v>
           </cell>
@@ -506,8 +559,17 @@
             <v>0</v>
           </cell>
           <cell r="M11">
+            <v>0</v>
+          </cell>
+          <cell r="N11">
             <v>81</v>
           </cell>
+          <cell r="O11"/>
+          <cell r="P11"/>
+          <cell r="Q11"/>
+          <cell r="R11"/>
+          <cell r="S11"/>
+          <cell r="T11"/>
         </row>
       </sheetData>
       <sheetData sheetId="5">
@@ -561,24 +623,31 @@
           <cell r="I8" t="str">
             <v>Somatória dos setores</v>
           </cell>
-          <cell r="J8">
+          <cell r="J8"/>
+          <cell r="K8">
             <v>18</v>
           </cell>
-          <cell r="K8">
+          <cell r="L8">
             <v>35</v>
           </cell>
-          <cell r="L8">
+          <cell r="M8">
             <v>36</v>
           </cell>
-          <cell r="M8">
+          <cell r="N8">
             <v>23</v>
           </cell>
-          <cell r="N8">
+          <cell r="O8">
             <v>34</v>
           </cell>
-          <cell r="O8">
+          <cell r="P8">
             <v>37</v>
           </cell>
+          <cell r="Q8"/>
+          <cell r="R8"/>
+          <cell r="S8"/>
+          <cell r="T8"/>
+          <cell r="U8"/>
+          <cell r="V8"/>
         </row>
       </sheetData>
     </sheetDataSet>
@@ -1134,11 +1203,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2645D7F8-92DB-4E6C-9667-0835191EABDE}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1160,217 +1227,181 @@
         <v>Cliente</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D2" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>5</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C3" s="1">
         <v>22</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>10</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="1">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D4" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="1">
         <v>16</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D5" s="1">
         <v>13</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="1">
         <v>8</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="1">
         <v>12</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="1">
         <v>9</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>9</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B8" s="1">
         <v>14</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="1">
         <v>7</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="1">
         <v>15</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B13" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C13" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D13" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D13" s="1" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1379,7 +1410,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277F78E7-0AEF-48AC-B99D-3738C29C304B}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1406,89 +1437,23 @@
         <v>Vitória</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <f>[1]Envios!B3</f>
         <v>100</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <f>[1]Envios!C3</f>
         <v>59</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <f>[1]Envios!D3</f>
         <v>61</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <f>[1]Envios!E3</f>
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1497,7 +1462,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986E08AE-9E15-44D6-86DC-8C09B531D17A}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -1510,7 +1475,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK(([1]Envios!$G$8:$S$11)),"",[1]Envios!$G$8:$S$11))</f>
+        <f t="array" ref="A1:D14">TRANSPOSE(IF(ISBLANK(([1]Envios!$G$8:$T$11)),"",[1]Envios!$G$8:$T$11))</f>
         <v>Bruna</v>
       </c>
       <c r="B1" s="3" t="str">
@@ -1524,28 +1489,28 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>36</v>
-      </c>
-      <c r="C2" s="1">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
+      <c r="A2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D2" s="1" t="str">
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1555,13 +1520,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -1571,13 +1536,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1587,13 +1552,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -1603,32 +1568,32 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B8" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D8" s="1" t="str">
-        <v/>
+      <c r="A8" s="1">
+        <v>100</v>
+      </c>
+      <c r="B8" s="1">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1">
+        <v>81</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1708,6 +1673,20 @@
         <v/>
       </c>
       <c r="D13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D14" s="1" t="str">
         <v/>
       </c>
     </row>
@@ -1761,32 +1740,32 @@
         <v>Comercial</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <f>[1]Erros!A3</f>
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <f>[1]Erros!B3</f>
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <f>[1]Erros!C3</f>
         <v>4</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <f>[1]Erros!D3</f>
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1">
         <f>[1]Erros!E3</f>
         <v>1</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <f>[1]Erros!F3</f>
         <v>25</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <f>[1]Erros!G3</f>
         <v>0</v>
       </c>
@@ -1812,74 +1791,76 @@
   <sheetData>
     <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:A13">TRANSPOSE(IF(ISBLANK([1]Erros!$I$8:$U$8),"",[1]Erros!$I$8:$U$8))</f>
+        <f t="array" ref="A1:A14">TRANSPOSE(IF(ISBLANK([1]Erros!$I$8:$V$8),"",[1]Erros!$I$8:$V$8))</f>
         <v>Somatória dos setores</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
adicionado media anual + formatação de exibição
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\Projetos\estatisticas_iten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\estatisticas_iten-main\estatisticas_iten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17D411A-65B1-4BAF-A782-210CE68228AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A835964-0AF9-4562-B748-BE01A1DCD47C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
+    <workbookView xWindow="0" yWindow="2340" windowWidth="28800" windowHeight="12180" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
   </bookViews>
   <sheets>
     <sheet name="atrasos" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
   <definedNames>
     <definedName name="Setor">[1]Atrasos!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,12 +36,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,14 +44,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -71,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Eletrodoméstico</t>
   </si>
@@ -101,6 +96,9 @@
   </si>
   <si>
     <t>Clientes</t>
+  </si>
+  <si>
+    <t>Construção Civil</t>
   </si>
 </sst>
 </file>
@@ -181,11 +179,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Sheet1"/>
       <sheetName val="config"/>
@@ -200,82 +195,87 @@
       <sheetData sheetId="2">
         <row r="3">
           <cell r="L3">
-            <v>24</v>
+            <v>19</v>
           </cell>
         </row>
         <row r="5">
           <cell r="L5">
-            <v>49</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="7">
           <cell r="L7">
-            <v>63</v>
+            <v>39</v>
           </cell>
         </row>
         <row r="9">
           <cell r="L9">
-            <v>4</v>
+            <v>33</v>
           </cell>
         </row>
         <row r="11">
           <cell r="L11">
-            <v>1</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="13">
           <cell r="L13">
-            <v>10</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="15">
           <cell r="L15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="N41" t="str">
-            <v>REP</v>
-          </cell>
-          <cell r="P41">
-            <v>8</v>
-          </cell>
-          <cell r="Q41">
-            <v>8</v>
-          </cell>
-          <cell r="R41">
-            <v>2</v>
-          </cell>
-          <cell r="S41">
-            <v>7</v>
-          </cell>
-          <cell r="T41">
-            <v>4</v>
-          </cell>
-          <cell r="U41">
-            <v>26</v>
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="L17">
+            <v>1</v>
           </cell>
         </row>
         <row r="42">
           <cell r="N42" t="str">
+            <v>REP</v>
+          </cell>
+          <cell r="P42">
+            <v>8</v>
+          </cell>
+          <cell r="Q42">
+            <v>8</v>
+          </cell>
+          <cell r="R42">
+            <v>2</v>
+          </cell>
+          <cell r="S42">
+            <v>7</v>
+          </cell>
+          <cell r="T42">
+            <v>4</v>
+          </cell>
+          <cell r="U42">
+            <v>26</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="N43" t="str">
             <v>Técnico</v>
           </cell>
-          <cell r="P42">
+          <cell r="P43">
             <v>33</v>
           </cell>
-          <cell r="Q42">
+          <cell r="Q43">
             <v>25</v>
           </cell>
-          <cell r="R42">
+          <cell r="R43">
             <v>32</v>
           </cell>
-          <cell r="S42">
+          <cell r="S43">
             <v>54</v>
           </cell>
-          <cell r="T42">
+          <cell r="T43">
             <v>74</v>
           </cell>
-          <cell r="U42">
+          <cell r="U43">
             <v>60</v>
           </cell>
         </row>
@@ -299,22 +299,22 @@
           <cell r="F8" t="str">
             <v>REP</v>
           </cell>
-          <cell r="G8">
+          <cell r="H8">
             <v>5</v>
           </cell>
-          <cell r="H8">
+          <cell r="I8">
             <v>10</v>
           </cell>
-          <cell r="I8">
+          <cell r="J8">
             <v>2</v>
           </cell>
-          <cell r="J8">
+          <cell r="K8">
             <v>6</v>
           </cell>
-          <cell r="K8">
+          <cell r="L8">
             <v>11</v>
           </cell>
-          <cell r="L8">
+          <cell r="M8">
             <v>9</v>
           </cell>
         </row>
@@ -322,22 +322,22 @@
           <cell r="F9" t="str">
             <v>Técnico</v>
           </cell>
-          <cell r="G9">
+          <cell r="H9">
             <v>10</v>
           </cell>
-          <cell r="H9">
+          <cell r="I9">
             <v>7</v>
           </cell>
-          <cell r="I9">
+          <cell r="J9">
             <v>16</v>
           </cell>
-          <cell r="J9">
+          <cell r="K9">
             <v>4</v>
           </cell>
-          <cell r="K9">
+          <cell r="L9">
             <v>12</v>
           </cell>
-          <cell r="L9">
+          <cell r="M9">
             <v>14</v>
           </cell>
         </row>
@@ -345,22 +345,22 @@
           <cell r="F10" t="str">
             <v>Comercial</v>
           </cell>
-          <cell r="G10">
+          <cell r="H10">
             <v>22</v>
           </cell>
-          <cell r="H10">
+          <cell r="I10">
             <v>6</v>
           </cell>
-          <cell r="I10">
+          <cell r="J10">
             <v>2</v>
           </cell>
-          <cell r="J10">
+          <cell r="K10">
             <v>3</v>
           </cell>
-          <cell r="K10">
+          <cell r="L10">
             <v>2</v>
           </cell>
-          <cell r="L10">
+          <cell r="M10">
             <v>7</v>
           </cell>
         </row>
@@ -368,22 +368,22 @@
           <cell r="F11" t="str">
             <v>Cliente</v>
           </cell>
-          <cell r="G11">
+          <cell r="H11">
             <v>14</v>
           </cell>
-          <cell r="H11">
+          <cell r="I11">
             <v>10</v>
           </cell>
-          <cell r="I11">
+          <cell r="J11">
             <v>13</v>
           </cell>
-          <cell r="J11">
+          <cell r="K11">
             <v>8</v>
           </cell>
-          <cell r="K11">
+          <cell r="L11">
             <v>9</v>
           </cell>
-          <cell r="L11">
+          <cell r="M11">
             <v>15</v>
           </cell>
         </row>
@@ -405,99 +405,90 @@
         </row>
         <row r="3">
           <cell r="B3">
+            <v>101</v>
+          </cell>
+          <cell r="C3">
+            <v>60</v>
+          </cell>
+          <cell r="D3">
+            <v>60</v>
+          </cell>
+          <cell r="E3">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="I8" t="str">
+            <v>Bruna</v>
+          </cell>
+          <cell r="K8">
+            <v>5</v>
+          </cell>
+          <cell r="L8">
+            <v>13</v>
+          </cell>
+          <cell r="M8">
+            <v>19</v>
+          </cell>
+          <cell r="N8">
+            <v>13</v>
+          </cell>
+          <cell r="O8">
+            <v>136</v>
+          </cell>
+          <cell r="P8">
             <v>100</v>
           </cell>
-          <cell r="C3">
+        </row>
+        <row r="9">
+          <cell r="I9" t="str">
+            <v>Elias</v>
+          </cell>
+          <cell r="K9">
+            <v>36</v>
+          </cell>
+          <cell r="L9">
+            <v>37</v>
+          </cell>
+          <cell r="M9">
+            <v>43</v>
+          </cell>
+          <cell r="N9">
+            <v>50</v>
+          </cell>
+          <cell r="O9">
+            <v>65</v>
+          </cell>
+          <cell r="P9">
             <v>59</v>
           </cell>
-          <cell r="D3">
+        </row>
+        <row r="10">
+          <cell r="I10" t="str">
+            <v>Marcel</v>
+          </cell>
+          <cell r="K10">
+            <v>11</v>
+          </cell>
+          <cell r="L10">
+            <v>29</v>
+          </cell>
+          <cell r="M10">
+            <v>46</v>
+          </cell>
+          <cell r="N10">
+            <v>28</v>
+          </cell>
+          <cell r="O10">
+            <v>127</v>
+          </cell>
+          <cell r="P10">
             <v>61</v>
           </cell>
-          <cell r="E3">
-            <v>81</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="G8" t="str">
-            <v>Bruna</v>
-          </cell>
-          <cell r="H8">
-            <v>5</v>
-          </cell>
-          <cell r="I8">
-            <v>13</v>
-          </cell>
-          <cell r="J8">
-            <v>19</v>
-          </cell>
-          <cell r="K8">
-            <v>13</v>
-          </cell>
-          <cell r="L8">
-            <v>136</v>
-          </cell>
-          <cell r="M8">
-            <v>100</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="G9" t="str">
-            <v>Elias</v>
-          </cell>
-          <cell r="H9">
-            <v>36</v>
-          </cell>
-          <cell r="I9">
-            <v>37</v>
-          </cell>
-          <cell r="J9">
-            <v>43</v>
-          </cell>
-          <cell r="K9">
-            <v>50</v>
-          </cell>
-          <cell r="L9">
-            <v>65</v>
-          </cell>
-          <cell r="M9">
-            <v>59</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="G10" t="str">
-            <v>Marcel</v>
-          </cell>
-          <cell r="H10">
-            <v>11</v>
-          </cell>
-          <cell r="I10">
-            <v>29</v>
-          </cell>
-          <cell r="J10">
-            <v>46</v>
-          </cell>
-          <cell r="K10">
-            <v>28</v>
-          </cell>
-          <cell r="L10">
-            <v>127</v>
-          </cell>
-          <cell r="M10">
-            <v>61</v>
-          </cell>
         </row>
         <row r="11">
-          <cell r="G11" t="str">
-            <v>Vitoria</v>
-          </cell>
-          <cell r="H11">
-            <v>0</v>
-          </cell>
-          <cell r="I11">
-            <v>0</v>
-          </cell>
-          <cell r="J11">
-            <v>0</v>
+          <cell r="I11" t="str">
+            <v>Vitória</v>
           </cell>
           <cell r="K11">
             <v>0</v>
@@ -506,7 +497,26 @@
             <v>0</v>
           </cell>
           <cell r="M11">
+            <v>0</v>
+          </cell>
+          <cell r="N11">
+            <v>0</v>
+          </cell>
+          <cell r="O11">
+            <v>0</v>
+          </cell>
+          <cell r="P11">
             <v>81</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="I12" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="I13" t="str">
+            <v/>
           </cell>
         </row>
       </sheetData>
@@ -525,12 +535,15 @@
             <v>Fogo</v>
           </cell>
           <cell r="E2" t="str">
+            <v>Construção Civil</v>
+          </cell>
+          <cell r="F2" t="str">
             <v>Plugues</v>
           </cell>
-          <cell r="F2" t="str">
+          <cell r="G2" t="str">
             <v>Eletrodoméstico</v>
           </cell>
-          <cell r="G2" t="str">
+          <cell r="H2" t="str">
             <v>Comercial</v>
           </cell>
         </row>
@@ -548,12 +561,15 @@
             <v>1</v>
           </cell>
           <cell r="E3">
+            <v>2</v>
+          </cell>
+          <cell r="F3">
             <v>1</v>
           </cell>
-          <cell r="F3">
+          <cell r="G3">
             <v>25</v>
           </cell>
-          <cell r="G3">
+          <cell r="H3">
             <v>0</v>
           </cell>
         </row>
@@ -561,22 +577,22 @@
           <cell r="I8" t="str">
             <v>Somatória dos setores</v>
           </cell>
-          <cell r="J8">
+          <cell r="K8">
             <v>18</v>
           </cell>
-          <cell r="K8">
+          <cell r="L8">
             <v>35</v>
           </cell>
-          <cell r="L8">
+          <cell r="M8">
             <v>36</v>
           </cell>
-          <cell r="M8">
+          <cell r="N8">
             <v>23</v>
           </cell>
-          <cell r="N8">
+          <cell r="O8">
             <v>34</v>
           </cell>
-          <cell r="O8">
+          <cell r="P8">
             <v>37</v>
           </cell>
         </row>
@@ -884,18 +900,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73481FEF-1CEE-46BB-90D1-F65A112B7DA0}">
   <sheetPr codeName="Planilha6"/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
-    <col min="2" max="7" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="8" width="18.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -912,40 +929,47 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>[1]Atrasos!L3</f>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <f>[1]Atrasos!L5</f>
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
         <f>[1]Atrasos!L7</f>
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D2" s="1">
         <f>[1]Atrasos!L9</f>
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1">
         <f>[1]Atrasos!L11</f>
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1">
         <f>[1]Atrasos!L13</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
         <f>[1]Atrasos!L15</f>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="H2" s="1">
+        <f>[1]Atrasos!L17</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -955,6 +979,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3DCFD-4B45-4DD1-B06F-B53AD002CBA5}">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -966,8 +991,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:B14">TRANSPOSE(IF(ISBLANK([1]Atrasos!$N$41:$AA$42),"",[1]Atrasos!$N$41:$AA$42))</f>
+      <c r="A1" s="3" t="str">
+        <f t="array" ref="A1:B14">TRANSPOSE(IF(ISBLANK([1]Atrasos!$N$42:$AA$42),"",[1]Atrasos!$N$42:$AA$43))</f>
         <v>REP</v>
       </c>
       <c r="B1" s="3" t="str">
@@ -1086,6 +1111,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4EA97A-E855-461E-8A3D-CEA2F63697DC}">
+  <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1134,11 +1160,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2645D7F8-92DB-4E6C-9667-0835191EABDE}">
+  <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1147,7 +1172,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK([1]Revisões!$F$8:$R$11),"",[1]Revisões!$F$8:$R$11))</f>
+        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK([1]Revisões!$F$8:$S$11),"",[1]Revisões!$F$8:$S$11))</f>
         <v>REP</v>
       </c>
       <c r="B1" s="3" t="str">
@@ -1161,105 +1186,105 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4">
-        <v>22</v>
-      </c>
-      <c r="D2" s="4">
-        <v>14</v>
+      <c r="A2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
         <v>10</v>
       </c>
-      <c r="B3" s="4">
-        <v>7</v>
-      </c>
       <c r="C3" s="4">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
         <v>9</v>
       </c>
-      <c r="B7" s="4">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4">
         <v>14</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="4">
         <v>7</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <v>15</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v/>
       </c>
       <c r="E8" s="4"/>
     </row>
@@ -1379,6 +1404,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277F78E7-0AEF-48AC-B99D-3738C29C304B}">
+  <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1408,20 +1434,20 @@
     </row>
     <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <f>[1]Envios!B3</f>
-        <v>100</v>
+        <f ca="1">[1]Envios!B3</f>
+        <v>101</v>
       </c>
       <c r="B2" s="4">
-        <f>[1]Envios!C3</f>
-        <v>59</v>
+        <f ca="1">[1]Envios!C3</f>
+        <v>60</v>
       </c>
       <c r="C2" s="4">
-        <f>[1]Envios!D3</f>
-        <v>61</v>
+        <f ca="1">[1]Envios!D3</f>
+        <v>60</v>
       </c>
       <c r="D2" s="4">
-        <f>[1]Envios!E3</f>
-        <v>81</v>
+        <f ca="1">[1]Envios!E3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1497,11 +1523,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986E08AE-9E15-44D6-86DC-8C09B531D17A}">
+  <sheetPr codeName="Planilha5"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1509,8 +1534,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK(([1]Envios!$G$8:$S$11)),"",[1]Envios!$G$8:$S$11))</f>
+      <c r="A1" s="3" t="str">
+        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK(([1]Envios!$I$8:$V$13)),"",[1]Envios!$I$8:$V$13))</f>
         <v>Bruna</v>
       </c>
       <c r="B1" s="3" t="str">
@@ -1520,32 +1545,32 @@
         <v>Marcel</v>
       </c>
       <c r="D1" s="3" t="str">
-        <v>Vitoria</v>
+        <v>Vitória</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>36</v>
-      </c>
-      <c r="C2" s="1">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
+      <c r="A2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D2" s="1" t="str">
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1555,13 +1580,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -1571,13 +1596,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -1587,13 +1612,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
-        <v>127</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -1603,32 +1628,32 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B8" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C8" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D8" s="1" t="str">
-        <v/>
+      <c r="A8" s="1">
+        <v>100</v>
+      </c>
+      <c r="B8" s="1">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1">
+        <v>61</v>
+      </c>
+      <c r="D8" s="1">
+        <v>81</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1718,20 +1743,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5EE03BC-37B0-46A8-9BC1-6D9C7D0B208A}">
-  <dimension ref="A1:G2"/>
+  <sheetPr codeName="Planilha7"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="18.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="10" width="18.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str">
         <f>[1]Erros!A2</f>
         <v>Cabos</v>
@@ -1750,18 +1773,22 @@
       </c>
       <c r="E1" s="3" t="str">
         <f>[1]Erros!E2</f>
-        <v>Plugues</v>
+        <v>Construção Civil</v>
       </c>
       <c r="F1" s="3" t="str">
         <f>[1]Erros!F2</f>
-        <v>Eletrodoméstico</v>
+        <v>Plugues</v>
       </c>
       <c r="G1" s="3" t="str">
         <f>[1]Erros!G2</f>
+        <v>Eletrodoméstico</v>
+      </c>
+      <c r="H1" s="3" t="str">
+        <f>[1]Erros!H2</f>
         <v>Comercial</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <f>[1]Erros!A3</f>
         <v>4</v>
@@ -1780,24 +1807,30 @@
       </c>
       <c r="E2" s="4">
         <f>[1]Erros!E3</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4">
         <f>[1]Erros!F3</f>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G2" s="4">
         <f>[1]Erros!G3</f>
+        <v>25</v>
+      </c>
+      <c r="H2" s="4">
+        <f>[1]Erros!H3</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EFDAF4-BC35-4FAC-901E-DC11DDCF549E}">
+  <sheetPr codeName="Planilha8"/>
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1812,43 +1845,43 @@
   <sheetData>
     <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:A13">TRANSPOSE(IF(ISBLANK([1]Erros!$I$8:$U$8),"",[1]Erros!$I$8:$U$8))</f>
+        <f t="array" ref="A1:A13">TRANSPOSE(IF(ISBLANK([1]Erros!$I$8:$V$8),"",[1]Erros!$I$8:$V$8))</f>
         <v>Somatória dos setores</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>18</v>
+      <c r="A2" s="4" t="str">
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="str">
-        <v/>
       </c>
     </row>
     <row r="9" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
correção na media atual e atualização
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\estatisticas_iten-main\estatisticas_iten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A835964-0AF9-4562-B748-BE01A1DCD47C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0159B5-8488-47EF-B6CE-0DB8D5CAF0FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2340" windowWidth="28800" windowHeight="12180" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
   </bookViews>
   <sheets>
     <sheet name="atrasos" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,10 +157,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -195,27 +191,27 @@
       <sheetData sheetId="2">
         <row r="3">
           <cell r="L3">
-            <v>19</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="5">
           <cell r="L5">
-            <v>40</v>
+            <v>29</v>
           </cell>
         </row>
         <row r="7">
           <cell r="L7">
-            <v>39</v>
+            <v>28</v>
           </cell>
         </row>
         <row r="9">
           <cell r="L9">
-            <v>33</v>
+            <v>22</v>
           </cell>
         </row>
         <row r="11">
           <cell r="L11">
-            <v>40</v>
+            <v>28</v>
           </cell>
         </row>
         <row r="13">
@@ -225,7 +221,7 @@
         </row>
         <row r="15">
           <cell r="L15">
-            <v>5</v>
+            <v>3</v>
           </cell>
         </row>
         <row r="17">
@@ -253,7 +249,7 @@
             <v>4</v>
           </cell>
           <cell r="U42">
-            <v>26</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="43">
@@ -276,7 +272,7 @@
             <v>74</v>
           </cell>
           <cell r="U43">
-            <v>60</v>
+            <v>111</v>
           </cell>
         </row>
       </sheetData>
@@ -437,7 +433,7 @@
             <v>136</v>
           </cell>
           <cell r="P8">
-            <v>100</v>
+            <v>101</v>
           </cell>
         </row>
         <row r="9">
@@ -460,7 +456,7 @@
             <v>65</v>
           </cell>
           <cell r="P9">
-            <v>59</v>
+            <v>60</v>
           </cell>
         </row>
         <row r="10">
@@ -483,7 +479,7 @@
             <v>127</v>
           </cell>
           <cell r="P10">
-            <v>61</v>
+            <v>60</v>
           </cell>
         </row>
         <row r="11">
@@ -506,7 +502,7 @@
             <v>0</v>
           </cell>
           <cell r="P11">
-            <v>81</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="12">
@@ -593,7 +589,7 @@
             <v>34</v>
           </cell>
           <cell r="P8">
-            <v>37</v>
+            <v>39</v>
           </cell>
         </row>
       </sheetData>
@@ -902,7 +898,7 @@
   <sheetPr codeName="Planilha6"/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -941,23 +937,23 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>[1]Atrasos!L3</f>
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1">
         <f>[1]Atrasos!L5</f>
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1">
         <f>[1]Atrasos!L7</f>
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1">
         <f>[1]Atrasos!L9</f>
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1">
         <f>[1]Atrasos!L11</f>
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1">
         <f>[1]Atrasos!L13</f>
@@ -965,7 +961,7 @@
       </c>
       <c r="G2" s="1">
         <f>[1]Atrasos!L15</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1">
         <f>[1]Atrasos!L17</f>
@@ -992,7 +988,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str">
-        <f t="array" ref="A1:B14">TRANSPOSE(IF(ISBLANK([1]Atrasos!$N$42:$AA$42),"",[1]Atrasos!$N$42:$AA$43))</f>
+        <f t="array" ref="A1:B14">TRANSPOSE(IF(ISBLANK([1]Atrasos!$N$42:$AA$43),"",[1]Atrasos!$N$42:$AA$43))</f>
         <v>REP</v>
       </c>
       <c r="B1" s="3" t="str">
@@ -1049,10 +1045,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1">
-        <v>60</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1161,9 +1157,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2645D7F8-92DB-4E6C-9667-0835191EABDE}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1185,217 +1183,181 @@
         <v>Cliente</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D2" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>5</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>10</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>22</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>10</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>7</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>16</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>13</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>8</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>11</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>12</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>9</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>14</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>7</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>15</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D9" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D11" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <v/>
-      </c>
-      <c r="B13" s="4" t="str">
-        <v/>
-      </c>
-      <c r="C13" s="4" t="str">
-        <v/>
-      </c>
-      <c r="D13" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D9" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D10" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D13" s="1" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1405,7 +1367,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277F78E7-0AEF-48AC-B99D-3738C29C304B}">
   <sheetPr codeName="Planilha4"/>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1432,89 +1394,23 @@
         <v>Vitória</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <f ca="1">[1]Envios!B3</f>
         <v>101</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <f ca="1">[1]Envios!C3</f>
         <v>60</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <f ca="1">[1]Envios!D3</f>
         <v>60</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <f ca="1">[1]Envios!E3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1644,16 +1540,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1788,36 +1684,36 @@
         <v>Comercial</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <f>[1]Erros!A3</f>
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="1">
         <f>[1]Erros!B3</f>
         <v>2</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <f>[1]Erros!C3</f>
         <v>4</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <f>[1]Erros!D3</f>
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1">
         <f>[1]Erros!E3</f>
         <v>2</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="1">
         <f>[1]Erros!F3</f>
         <v>1</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <f>[1]Erros!G3</f>
         <v>25</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="1">
         <f>[1]Erros!H3</f>
         <v>0</v>
       </c>
@@ -1831,9 +1727,9 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EFDAF4-BC35-4FAC-901E-DC11DDCF549E}">
   <sheetPr codeName="Planilha8"/>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1849,70 +1745,66 @@
         <v>Somatória dos setores</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
correções de pequenos erros
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\estatisticas_iten-main\estatisticas_iten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0159B5-8488-47EF-B6CE-0DB8D5CAF0FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211A8750-3EDC-4A66-9FE3-A9378A078314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
   </bookViews>
   <sheets>
     <sheet name="atrasos" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="envios2" sheetId="7" r:id="rId6"/>
     <sheet name="erros" sheetId="8" r:id="rId7"/>
     <sheet name="erros2" sheetId="9" r:id="rId8"/>
+    <sheet name="info" sheetId="10" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="Setor">[1]Atrasos!#REF!</definedName>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Eletrodoméstico</t>
   </si>
@@ -99,6 +100,12 @@
   </si>
   <si>
     <t>Construção Civil</t>
+  </si>
+  <si>
+    <t>#mes</t>
+  </si>
+  <si>
+    <t>#ano</t>
   </si>
 </sst>
 </file>
@@ -148,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,6 +163,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -187,31 +200,42 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="10">
+          <cell r="B10">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>2023</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="2">
         <row r="3">
           <cell r="L3">
-            <v>55</v>
+            <v>41</v>
           </cell>
         </row>
         <row r="5">
           <cell r="L5">
-            <v>29</v>
+            <v>22</v>
           </cell>
         </row>
         <row r="7">
           <cell r="L7">
-            <v>28</v>
+            <v>21</v>
           </cell>
         </row>
         <row r="9">
           <cell r="L9">
-            <v>22</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="11">
           <cell r="L11">
-            <v>28</v>
+            <v>22</v>
           </cell>
         </row>
         <row r="13">
@@ -249,7 +273,7 @@
             <v>4</v>
           </cell>
           <cell r="U42">
-            <v>55</v>
+            <v>41</v>
           </cell>
         </row>
         <row r="43">
@@ -272,7 +296,7 @@
             <v>74</v>
           </cell>
           <cell r="U43">
-            <v>111</v>
+            <v>84</v>
           </cell>
         </row>
       </sheetData>
@@ -898,7 +922,7 @@
   <sheetPr codeName="Planilha6"/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -937,23 +961,23 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>[1]Atrasos!L3</f>
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1">
         <f>[1]Atrasos!L5</f>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1">
         <f>[1]Atrasos!L7</f>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <f>[1]Atrasos!L9</f>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1">
         <f>[1]Atrasos!L11</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1">
         <f>[1]Atrasos!L13</f>
@@ -1045,10 +1069,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1">
-        <v>111</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1729,7 +1753,7 @@
   <sheetPr codeName="Planilha8"/>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1808,4 +1832,41 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24AF4B41-D954-4754-AF3B-A1871C72B66B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <f>[1]config!$B$10</f>
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <f>[1]config!$B$13</f>
+        <v>2023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
att desempenho remov seleções
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\estatisticas_iten-main\estatisticas_iten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\estatisticas_iten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211A8750-3EDC-4A66-9FE3-A9378A078314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1934AF-17EA-4E3D-A48D-3198A3573665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
   </bookViews>
   <sheets>
     <sheet name="atrasos" sheetId="1" r:id="rId1"/>
@@ -155,16 +155,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -411,35 +408,47 @@
       <sheetData sheetId="4">
         <row r="2">
           <cell r="B2" t="str">
-            <v>Bruna</v>
+            <v>Marcel</v>
           </cell>
           <cell r="C2" t="str">
             <v>Elias</v>
           </cell>
           <cell r="D2" t="str">
-            <v>Marcel</v>
+            <v>Vitoria</v>
           </cell>
           <cell r="E2" t="str">
-            <v>Vitória</v>
+            <v>Bruna</v>
+          </cell>
+          <cell r="F2" t="str">
+            <v>Milena</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>101</v>
+            <v>60</v>
           </cell>
           <cell r="C3">
             <v>60</v>
           </cell>
           <cell r="D3">
-            <v>60</v>
+            <v>78</v>
           </cell>
           <cell r="E3">
-            <v>0</v>
+            <v>101</v>
+          </cell>
+          <cell r="F3">
+            <v>1</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v/>
+          </cell>
+          <cell r="H3" t="str">
+            <v/>
           </cell>
         </row>
         <row r="8">
           <cell r="I8" t="str">
-            <v>Bruna</v>
+            <v>Marcel</v>
           </cell>
           <cell r="K8">
             <v>5</v>
@@ -457,7 +466,7 @@
             <v>136</v>
           </cell>
           <cell r="P8">
-            <v>101</v>
+            <v>60</v>
           </cell>
         </row>
         <row r="9">
@@ -485,7 +494,7 @@
         </row>
         <row r="10">
           <cell r="I10" t="str">
-            <v>Marcel</v>
+            <v>Vitoria</v>
           </cell>
           <cell r="K10">
             <v>11</v>
@@ -503,12 +512,12 @@
             <v>127</v>
           </cell>
           <cell r="P10">
-            <v>60</v>
+            <v>78</v>
           </cell>
         </row>
         <row r="11">
           <cell r="I11" t="str">
-            <v>Vitória</v>
+            <v>Bruna</v>
           </cell>
           <cell r="K11">
             <v>0</v>
@@ -526,16 +535,21 @@
             <v>0</v>
           </cell>
           <cell r="P11">
-            <v>0</v>
+            <v>101</v>
           </cell>
         </row>
         <row r="12">
           <cell r="I12" t="str">
-            <v/>
+            <v>Milena</v>
           </cell>
         </row>
         <row r="13">
           <cell r="I13" t="str">
+            <v/>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="I14" t="str">
             <v/>
           </cell>
         </row>
@@ -922,7 +936,7 @@
   <sheetPr codeName="Planilha6"/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1181,7 +1195,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2645D7F8-92DB-4E6C-9667-0835191EABDE}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
@@ -1194,7 +1208,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK([1]Revisões!$F$8:$S$11),"",[1]Revisões!$F$8:$S$11))</f>
+        <f t="array" ref="A1:D14">TRANSPOSE(IF(ISBLANK([1]Revisões!$F$8:$S$11),"",[1]Revisões!$F$8:$S$11))</f>
         <v>REP</v>
       </c>
       <c r="B1" s="3" t="str">
@@ -1380,6 +1394,20 @@
         <v/>
       </c>
       <c r="D13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="B14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="C14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D14" s="1" t="str">
         <v/>
       </c>
     </row>
@@ -1391,49 +1419,76 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277F78E7-0AEF-48AC-B99D-3738C29C304B}">
   <sheetPr codeName="Planilha4"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="1" max="4" width="18.7109375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str">
-        <f>[1]Envios!B2</f>
+        <f>IF([1]Envios!B2="","",[1]Envios!B2)</f>
+        <v>Marcel</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <f>IF([1]Envios!C2="","",[1]Envios!C2)</f>
+        <v>Elias</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <f>IF([1]Envios!D2="","",[1]Envios!D2)</f>
+        <v>Vitoria</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <f>IF([1]Envios!E2="","",[1]Envios!E2)</f>
         <v>Bruna</v>
       </c>
-      <c r="B1" s="3" t="str">
-        <f>[1]Envios!C2</f>
-        <v>Elias</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <f>[1]Envios!D2</f>
-        <v>Marcel</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <f>[1]Envios!E2</f>
-        <v>Vitória</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="str">
+        <f>IF([1]Envios!F2="","",[1]Envios!F2)</f>
+        <v>Milena</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <f>IF([1]Envios!G2="","",[1]Envios!G2)</f>
+        <v/>
+      </c>
+      <c r="G1" s="3" t="str">
+        <f>IF([1]Envios!H2="","",[1]Envios!H2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f ca="1">[1]Envios!B3</f>
+        <f ca="1">IF([1]Envios!B3="","",[1]Envios!B3)</f>
+        <v>60</v>
+      </c>
+      <c r="B2" s="1">
+        <f ca="1">IF([1]Envios!C3="","",[1]Envios!C3)</f>
+        <v>60</v>
+      </c>
+      <c r="C2" s="1">
+        <f ca="1">IF([1]Envios!D3="","",[1]Envios!D3)</f>
+        <v>78</v>
+      </c>
+      <c r="D2" s="1">
+        <f ca="1">IF([1]Envios!E3="","",[1]Envios!E3)</f>
         <v>101</v>
       </c>
-      <c r="B2" s="1">
-        <f ca="1">[1]Envios!C3</f>
-        <v>60</v>
-      </c>
-      <c r="C2" s="1">
-        <f ca="1">[1]Envios!D3</f>
-        <v>60</v>
-      </c>
-      <c r="D2" s="1">
-        <f ca="1">[1]Envios!E3</f>
-        <v>0</v>
+      <c r="E2" s="1">
+        <f ca="1">IF([1]Envios!F3="","",[1]Envios!F3)</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>IF([1]Envios!G3="","",[1]Envios!G3)</f>
+        <v/>
+      </c>
+      <c r="G2" s="1" t="str">
+        <f>IF([1]Envios!H3="","",[1]Envios!H3)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1446,7 +1501,9 @@
   <sheetPr codeName="Planilha5"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1455,17 +1512,17 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str">
-        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK(([1]Envios!$I$8:$V$13)),"",[1]Envios!$I$8:$V$13))</f>
-        <v>Bruna</v>
+        <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK(([1]Envios!$I$8:$V$14)),"",[1]Envios!$I$8:$V$14))</f>
+        <v>Marcel</v>
       </c>
       <c r="B1" s="3" t="str">
         <v>Elias</v>
       </c>
       <c r="C1" s="3" t="str">
-        <v>Marcel</v>
+        <v>Vitoria</v>
       </c>
       <c r="D1" s="3" t="str">
-        <v>Vitória</v>
+        <v>Bruna</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1564,16 +1621,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1">
         <v>60</v>
       </c>
       <c r="C8" s="1">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1751,7 +1808,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EFDAF4-BC35-4FAC-901E-DC11DDCF549E}">
   <sheetPr codeName="Planilha8"/>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1765,7 +1822,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str" cm="1">
-        <f t="array" ref="A1:A13">TRANSPOSE(IF(ISBLANK([1]Erros!$I$8:$V$8),"",[1]Erros!$I$8:$V$8))</f>
+        <f t="array" ref="A1:A14">TRANSPOSE(IF(ISBLANK([1]Erros!$I$8:$V$8),"",[1]Erros!$I$8:$V$8))</f>
         <v>Somatória dos setores</v>
       </c>
     </row>
@@ -1826,6 +1883,11 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
         <v/>
       </c>
     </row>
@@ -1836,6 +1898,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24AF4B41-D954-4754-AF3B-A1871C72B66B}">
+  <sheetPr codeName="Planilha9"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1844,8 +1907,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1857,11 +1920,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="1">
         <f>[1]config!$B$10</f>
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <f>[1]config!$B$13</f>
         <v>2023</v>
       </c>

</xml_diff>

<commit_message>
correção de erros + e - e exclusao do html
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\estatisticas_iten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFAB393-4A3B-4E10-AB3B-4298F72D3894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304CF237-E9CF-4B29-B6AD-9FCA9DCEF4F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA21E64C-BFD3-447A-A370-1138DFC2D88F}"/>
   </bookViews>
@@ -33,12 +33,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -200,7 +194,7 @@
       <sheetData sheetId="1">
         <row r="10">
           <cell r="B10">
-            <v>6</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="13">
@@ -212,42 +206,42 @@
       <sheetData sheetId="2">
         <row r="3">
           <cell r="L3">
-            <v>41</v>
+            <v>54</v>
           </cell>
         </row>
         <row r="5">
           <cell r="L5">
-            <v>22</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="7">
           <cell r="L7">
-            <v>21</v>
+            <v>24</v>
           </cell>
         </row>
         <row r="9">
           <cell r="L9">
-            <v>15</v>
+            <v>27</v>
           </cell>
         </row>
         <row r="11">
           <cell r="L11">
-            <v>22</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="13">
           <cell r="L13">
-            <v>0</v>
+            <v>7</v>
           </cell>
         </row>
         <row r="15">
           <cell r="L15">
-            <v>3</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="17">
           <cell r="L17">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="42">
@@ -272,6 +266,18 @@
           <cell r="U42">
             <v>41</v>
           </cell>
+          <cell r="V42">
+            <v>21</v>
+          </cell>
+          <cell r="W42">
+            <v>10</v>
+          </cell>
+          <cell r="X42">
+            <v>31</v>
+          </cell>
+          <cell r="Y42">
+            <v>54</v>
+          </cell>
         </row>
         <row r="43">
           <cell r="N43" t="str">
@@ -294,22 +300,34 @@
           </cell>
           <cell r="U43">
             <v>84</v>
+          </cell>
+          <cell r="V43">
+            <v>33</v>
+          </cell>
+          <cell r="W43">
+            <v>47</v>
+          </cell>
+          <cell r="X43">
+            <v>101</v>
+          </cell>
+          <cell r="Y43">
+            <v>55</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
         <row r="3">
           <cell r="A3">
-            <v>9</v>
+            <v>4</v>
           </cell>
           <cell r="B3">
-            <v>14</v>
+            <v>19</v>
           </cell>
           <cell r="C3">
-            <v>7</v>
+            <v>12</v>
           </cell>
           <cell r="D3">
-            <v>15</v>
+            <v>44</v>
           </cell>
         </row>
         <row r="8">
@@ -334,6 +352,18 @@
           <cell r="M8">
             <v>9</v>
           </cell>
+          <cell r="N8">
+            <v>5</v>
+          </cell>
+          <cell r="O8">
+            <v>7</v>
+          </cell>
+          <cell r="P8">
+            <v>11</v>
+          </cell>
+          <cell r="Q8">
+            <v>4</v>
+          </cell>
         </row>
         <row r="9">
           <cell r="F9" t="str">
@@ -357,6 +387,18 @@
           <cell r="M9">
             <v>14</v>
           </cell>
+          <cell r="N9">
+            <v>9</v>
+          </cell>
+          <cell r="O9">
+            <v>3</v>
+          </cell>
+          <cell r="P9">
+            <v>12</v>
+          </cell>
+          <cell r="Q9">
+            <v>19</v>
+          </cell>
         </row>
         <row r="10">
           <cell r="F10" t="str">
@@ -380,6 +422,18 @@
           <cell r="M10">
             <v>7</v>
           </cell>
+          <cell r="N10">
+            <v>1</v>
+          </cell>
+          <cell r="O10">
+            <v>2</v>
+          </cell>
+          <cell r="P10">
+            <v>1</v>
+          </cell>
+          <cell r="Q10">
+            <v>12</v>
+          </cell>
         </row>
         <row r="11">
           <cell r="F11" t="str">
@@ -402,42 +456,51 @@
           </cell>
           <cell r="M11">
             <v>15</v>
+          </cell>
+          <cell r="N11">
+            <v>18</v>
+          </cell>
+          <cell r="O11">
+            <v>10</v>
+          </cell>
+          <cell r="P11">
+            <v>23</v>
+          </cell>
+          <cell r="Q11">
+            <v>44</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="4">
         <row r="2">
           <cell r="B2" t="str">
-            <v>Marcel</v>
+            <v>BRUNA</v>
           </cell>
           <cell r="C2" t="str">
-            <v>Elias</v>
+            <v>ELIAS</v>
           </cell>
           <cell r="D2" t="str">
-            <v>Vitoria</v>
+            <v>MARCEL</v>
           </cell>
           <cell r="E2" t="str">
-            <v>Bruna</v>
-          </cell>
-          <cell r="F2" t="str">
-            <v>Milena</v>
+            <v>VITORIA</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>60</v>
+            <v>82</v>
           </cell>
           <cell r="C3">
-            <v>60</v>
+            <v>74</v>
           </cell>
           <cell r="D3">
-            <v>78</v>
+            <v>41</v>
           </cell>
           <cell r="E3">
-            <v>101</v>
-          </cell>
-          <cell r="F3">
-            <v>1</v>
+            <v>98</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v/>
           </cell>
           <cell r="G3" t="str">
             <v/>
@@ -448,30 +511,42 @@
         </row>
         <row r="8">
           <cell r="I8" t="str">
-            <v>Marcel</v>
+            <v>BRUNA</v>
           </cell>
           <cell r="K8">
-            <v>11</v>
+            <v>5</v>
           </cell>
           <cell r="L8">
-            <v>29</v>
+            <v>13</v>
           </cell>
           <cell r="M8">
-            <v>46</v>
+            <v>19</v>
           </cell>
           <cell r="N8">
-            <v>28</v>
+            <v>13</v>
           </cell>
           <cell r="O8">
-            <v>127</v>
+            <v>136</v>
           </cell>
           <cell r="P8">
-            <v>60</v>
+            <v>101</v>
+          </cell>
+          <cell r="Q8">
+            <v>97</v>
+          </cell>
+          <cell r="R8">
+            <v>49</v>
+          </cell>
+          <cell r="S8">
+            <v>98</v>
+          </cell>
+          <cell r="T8">
+            <v>82</v>
           </cell>
         </row>
         <row r="9">
           <cell r="I9" t="str">
-            <v>Elias</v>
+            <v>ELIAS</v>
           </cell>
           <cell r="K9">
             <v>36</v>
@@ -491,41 +566,77 @@
           <cell r="P9">
             <v>60</v>
           </cell>
+          <cell r="Q9">
+            <v>64</v>
+          </cell>
+          <cell r="R9">
+            <v>60</v>
+          </cell>
+          <cell r="S9">
+            <v>55</v>
+          </cell>
+          <cell r="T9">
+            <v>74</v>
+          </cell>
         </row>
         <row r="10">
           <cell r="I10" t="str">
-            <v>Vitoria</v>
+            <v>MARCEL</v>
+          </cell>
+          <cell r="K10">
+            <v>11</v>
+          </cell>
+          <cell r="L10">
+            <v>29</v>
+          </cell>
+          <cell r="M10">
+            <v>46</v>
+          </cell>
+          <cell r="N10">
+            <v>28</v>
+          </cell>
+          <cell r="O10">
+            <v>127</v>
           </cell>
           <cell r="P10">
-            <v>78</v>
+            <v>60</v>
+          </cell>
+          <cell r="Q10">
+            <v>39</v>
+          </cell>
+          <cell r="R10">
+            <v>10</v>
+          </cell>
+          <cell r="S10">
+            <v>41</v>
+          </cell>
+          <cell r="T10">
+            <v>41</v>
           </cell>
         </row>
         <row r="11">
           <cell r="I11" t="str">
-            <v>Bruna</v>
-          </cell>
-          <cell r="K11">
-            <v>5</v>
-          </cell>
-          <cell r="L11">
-            <v>13</v>
-          </cell>
-          <cell r="M11">
-            <v>19</v>
-          </cell>
-          <cell r="N11">
-            <v>13</v>
-          </cell>
-          <cell r="O11">
-            <v>136</v>
+            <v>VITORIA</v>
           </cell>
           <cell r="P11">
-            <v>101</v>
+            <v>78</v>
+          </cell>
+          <cell r="Q11">
+            <v>60</v>
+          </cell>
+          <cell r="R11">
+            <v>77</v>
+          </cell>
+          <cell r="S11">
+            <v>98</v>
+          </cell>
+          <cell r="T11">
+            <v>98</v>
           </cell>
         </row>
         <row r="12">
           <cell r="I12" t="str">
-            <v>Milena</v>
+            <v/>
           </cell>
         </row>
         <row r="13">
@@ -568,28 +679,28 @@
         </row>
         <row r="3">
           <cell r="A3">
-            <v>4</v>
+            <v>0</v>
           </cell>
           <cell r="B3">
             <v>2</v>
           </cell>
           <cell r="C3">
-            <v>4</v>
+            <v>2</v>
           </cell>
           <cell r="D3">
+            <v>0</v>
+          </cell>
+          <cell r="E3">
+            <v>0</v>
+          </cell>
+          <cell r="F3">
+            <v>2</v>
+          </cell>
+          <cell r="G3">
+            <v>0</v>
+          </cell>
+          <cell r="H3">
             <v>1</v>
-          </cell>
-          <cell r="E3">
-            <v>2</v>
-          </cell>
-          <cell r="F3">
-            <v>1</v>
-          </cell>
-          <cell r="G3">
-            <v>25</v>
-          </cell>
-          <cell r="H3">
-            <v>0</v>
           </cell>
         </row>
         <row r="8">
@@ -612,7 +723,19 @@
             <v>34</v>
           </cell>
           <cell r="P8">
-            <v>39</v>
+            <v>37</v>
+          </cell>
+          <cell r="Q8">
+            <v>21</v>
+          </cell>
+          <cell r="R8">
+            <v>18</v>
+          </cell>
+          <cell r="S8">
+            <v>16</v>
+          </cell>
+          <cell r="T8">
+            <v>7</v>
           </cell>
         </row>
       </sheetData>
@@ -960,35 +1083,35 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>[1]Atrasos!L3</f>
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1">
         <f>[1]Atrasos!L5</f>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <f>[1]Atrasos!L7</f>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1">
         <f>[1]Atrasos!L9</f>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1">
         <f>[1]Atrasos!L11</f>
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1">
         <f>[1]Atrasos!L13</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1">
         <f>[1]Atrasos!L15</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1">
         <f>[1]Atrasos!L17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1075,35 +1198,35 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="str">
-        <v/>
-      </c>
-      <c r="B9" s="1" t="str">
-        <v/>
+      <c r="A9" s="3">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="str">
-        <v/>
-      </c>
-      <c r="B10" s="3" t="str">
-        <v/>
+      <c r="A10" s="3">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="str">
-        <v/>
-      </c>
-      <c r="B11" s="1" t="str">
-        <v/>
+      <c r="A11" s="3">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B12" s="1" t="str">
-        <v/>
+      <c r="A12" s="1">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1157,19 +1280,19 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>[1]Revisões!A3</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <f>[1]Revisões!B3</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <f>[1]Revisões!C3</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <f>[1]Revisões!D3</f>
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1310,62 +1433,62 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B9" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C9" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D9" s="1" t="str">
-        <v/>
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>18</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B10" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C10" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D10" s="1" t="str">
-        <v/>
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B11" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C11" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D11" s="1" t="str">
-        <v/>
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>23</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B12" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C12" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D12" s="1" t="str">
-        <v/>
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,23 +1542,23 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str">
         <f>IF([1]Envios!B2="","",[1]Envios!B2)</f>
-        <v>Marcel</v>
+        <v>BRUNA</v>
       </c>
       <c r="B1" s="3" t="str">
         <f>IF([1]Envios!C2="","",[1]Envios!C2)</f>
-        <v>Elias</v>
+        <v>ELIAS</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>IF([1]Envios!D2="","",[1]Envios!D2)</f>
-        <v>Vitoria</v>
+        <v>MARCEL</v>
       </c>
       <c r="D1" s="3" t="str">
         <f>IF([1]Envios!E2="","",[1]Envios!E2)</f>
-        <v>Bruna</v>
+        <v>VITORIA</v>
       </c>
       <c r="E1" s="3" t="str">
         <f>IF([1]Envios!F2="","",[1]Envios!F2)</f>
-        <v>Milena</v>
+        <v/>
       </c>
       <c r="F1" s="3" t="str">
         <f>IF([1]Envios!G2="","",[1]Envios!G2)</f>
@@ -1449,23 +1572,23 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f ca="1">IF([1]Envios!B3="","",[1]Envios!B3)</f>
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1">
         <f ca="1">IF([1]Envios!C3="","",[1]Envios!C3)</f>
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1">
         <f ca="1">IF([1]Envios!D3="","",[1]Envios!D3)</f>
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1">
         <f ca="1">IF([1]Envios!E3="","",[1]Envios!E3)</f>
-        <v>101</v>
-      </c>
-      <c r="E2" s="1">
-        <f ca="1">IF([1]Envios!F3="","",[1]Envios!F3)</f>
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>IF([1]Envios!F3="","",[1]Envios!F3)</f>
+        <v/>
       </c>
       <c r="F2" s="1" t="str">
         <f>IF([1]Envios!G3="","",[1]Envios!G3)</f>
@@ -1498,16 +1621,16 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="str">
         <f t="array" ref="A1:D13">TRANSPOSE(IF(ISBLANK(([1]Envios!$I$8:$V$14)),"",[1]Envios!$I$8:$V$14))</f>
-        <v>Marcel</v>
+        <v>BRUNA</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Elias</v>
+        <v>ELIAS</v>
       </c>
       <c r="C1" s="3" t="str">
-        <v>Vitoria</v>
+        <v>MARCEL</v>
       </c>
       <c r="D1" s="3" t="str">
-        <v>Bruna</v>
+        <v>VITORIA</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1526,160 +1649,160 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>36</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D3" s="1">
-        <v>5</v>
+      <c r="C3" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <v/>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D4" s="1">
-        <v>13</v>
+      <c r="C4" s="1">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <v/>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>43</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D5" s="1">
-        <v>19</v>
+      <c r="C5" s="1">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="str">
+        <v/>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>50</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D6" s="1">
-        <v>13</v>
+      <c r="C6" s="1">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <v/>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B7" s="1">
         <v>65</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D7" s="1">
-        <v>136</v>
+      <c r="C7" s="1">
+        <v>127</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <v/>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1">
         <v>60</v>
       </c>
       <c r="C8" s="1">
+        <v>60</v>
+      </c>
+      <c r="D8" s="1">
         <v>78</v>
-      </c>
-      <c r="D8" s="1">
-        <v>101</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B9" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C9" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D9" s="1" t="str">
-        <v/>
+      <c r="A9" s="1">
+        <v>97</v>
+      </c>
+      <c r="B9" s="1">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1">
+        <v>60</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B10" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C10" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D10" s="1" t="str">
-        <v/>
+      <c r="A10" s="1">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1">
+        <v>60</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1">
+        <v>77</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B11" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C11" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D11" s="1" t="str">
-        <v/>
+      <c r="A11" s="1">
+        <v>98</v>
+      </c>
+      <c r="B11" s="1">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1">
+        <v>98</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <v/>
-      </c>
-      <c r="B12" s="1" t="str">
-        <v/>
-      </c>
-      <c r="C12" s="1" t="str">
-        <v/>
-      </c>
-      <c r="D12" s="1" t="str">
-        <v/>
+      <c r="A12" s="1">
+        <v>82</v>
+      </c>
+      <c r="B12" s="1">
+        <v>74</v>
+      </c>
+      <c r="C12" s="1">
+        <v>41</v>
+      </c>
+      <c r="D12" s="1">
+        <v>98</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1753,7 +1876,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>[1]Erros!A3</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <f>[1]Erros!B3</f>
@@ -1761,27 +1884,27 @@
       </c>
       <c r="C2" s="1">
         <f>[1]Erros!C3</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <f>[1]Erros!D3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <f>[1]Erros!E3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <f>[1]Erros!F3</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
         <f>[1]Erros!G3</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
         <f>[1]Erros!H3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1843,27 +1966,27 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <v/>
+      <c r="A9" s="1">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <v/>
+      <c r="A10" s="1">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <v/>
+      <c r="A11" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <v/>
+      <c r="A12" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -1907,7 +2030,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>[1]config!$B$10</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4">
         <f>[1]config!$B$13</f>

</xml_diff>